<commit_message>
[up] start constructing final project
</commit_message>
<xml_diff>
--- a/FinalProject/Schedule.xlsx
+++ b/FinalProject/Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Windows_Storage\Storage\Github\softComputing\FinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{332A8881-6E16-4453-87BC-B0162BE474E6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25BDF3B2-C03E-495C-A6EE-0673A74EFEB8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9204" xr2:uid="{BB5E7CAA-F378-458D-ADC1-5DC4CD42EDC8}"/>
   </bookViews>
@@ -280,19 +280,19 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>43835</c:v>
+                  <c:v>44201</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43835</c:v>
+                  <c:v>44201</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43839</c:v>
+                  <c:v>44205</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43844</c:v>
+                  <c:v>44210</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43845</c:v>
+                  <c:v>44211</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -443,7 +443,7 @@
         <c:axId val="427418479"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="43835"/>
+          <c:min val="44200"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1451,7 +1451,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1473,7 +1473,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="1">
-        <v>43835</v>
+        <v>44201</v>
       </c>
       <c r="C2">
         <v>4</v>
@@ -1484,7 +1484,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1">
-        <v>43835</v>
+        <v>44201</v>
       </c>
       <c r="C3">
         <v>4</v>
@@ -1495,7 +1495,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="1">
-        <v>43839</v>
+        <v>44205</v>
       </c>
       <c r="C4">
         <v>5</v>
@@ -1506,7 +1506,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="1">
-        <v>43844</v>
+        <v>44210</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -1517,7 +1517,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="1">
-        <v>43845</v>
+        <v>44211</v>
       </c>
       <c r="C6">
         <v>3</v>

</xml_diff>